<commit_message>
creating the actual file for excel info
</commit_message>
<xml_diff>
--- a/display/smooth_region_coordinates.xlsx
+++ b/display/smooth_region_coordinates.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="33" uniqueCount="33">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="64" uniqueCount="64">
   <si>
     <t>Region</t>
   </si>
@@ -25,94 +25,187 @@
     <t>Area</t>
   </si>
   <si>
-    <t>(247, 9, 294, 32)</t>
-  </si>
-  <si>
-    <t>(194, 124, 227, 157)</t>
-  </si>
-  <si>
-    <t>(74, 124, 107, 157)</t>
-  </si>
-  <si>
-    <t>(247, 49, 294, 72)</t>
-  </si>
-  <si>
-    <t>(7, 329, 54, 352)</t>
-  </si>
-  <si>
-    <t>(247, 329, 294, 352)</t>
-  </si>
-  <si>
-    <t>(247, 89, 294, 112)</t>
-  </si>
-  <si>
-    <t>(7, 9, 54, 32)</t>
-  </si>
-  <si>
-    <t>(247, 149, 294, 172)</t>
-  </si>
-  <si>
-    <t>(7, 149, 54, 172)</t>
-  </si>
-  <si>
-    <t>(254, 184, 287, 217)</t>
-  </si>
-  <si>
-    <t>(4, 277, 27, 324)</t>
-  </si>
-  <si>
-    <t>(4, 177, 27, 224)</t>
-  </si>
-  <si>
-    <t>(259, 277, 282, 324)</t>
-  </si>
-  <si>
-    <t>(7, 369, 54, 392)</t>
-  </si>
-  <si>
-    <t>(274, 217, 297, 264)</t>
-  </si>
-  <si>
-    <t>(242, 111, 299, 130)</t>
-  </si>
-  <si>
-    <t>(247, 369, 294, 392)</t>
-  </si>
-  <si>
-    <t>(2, 131, 59, 150)</t>
-  </si>
-  <si>
-    <t>(242, 71, 299, 90)</t>
-  </si>
-  <si>
-    <t>(242, 131, 299, 150)</t>
-  </si>
-  <si>
-    <t>(2, 351, 59, 370)</t>
-  </si>
-  <si>
-    <t>(242, 351, 299, 370)</t>
-  </si>
-  <si>
-    <t>(242, 31, 299, 50)</t>
-  </si>
-  <si>
-    <t>(144, 375, 247, 386)</t>
-  </si>
-  <si>
-    <t>(114, 315, 217, 326)</t>
-  </si>
-  <si>
-    <t>(54, 373, 127, 388)</t>
-  </si>
-  <si>
-    <t>(14, 244, 47, 277)</t>
-  </si>
-  <si>
-    <t>(214, 157, 237, 204)</t>
-  </si>
-  <si>
-    <t>(64, 157, 87, 204)</t>
+    <t>Centroid</t>
+  </si>
+  <si>
+    <t>(37, 255, 84, 346)</t>
+  </si>
+  <si>
+    <t>(34, 350, 237, 371)</t>
+  </si>
+  <si>
+    <t>(34, 370, 237, 391)</t>
+  </si>
+  <si>
+    <t>(34, 30, 237, 51)</t>
+  </si>
+  <si>
+    <t>(89, 284, 122, 317)</t>
+  </si>
+  <si>
+    <t>(13, 188, 78, 253)</t>
+  </si>
+  <si>
+    <t>(239, 344, 272, 377)</t>
+  </si>
+  <si>
+    <t>(92, 331, 149, 350)</t>
+  </si>
+  <si>
+    <t>(19, 97, 42, 144)</t>
+  </si>
+  <si>
+    <t>(14, 144, 47, 177)</t>
+  </si>
+  <si>
+    <t>(19, 50, 222, 71)</t>
+  </si>
+  <si>
+    <t>(34, 10, 237, 31)</t>
+  </si>
+  <si>
+    <t>(89, 244, 122, 277)</t>
+  </si>
+  <si>
+    <t>(24, 73, 97, 88)</t>
+  </si>
+  <si>
+    <t>(152, 331, 209, 350)</t>
+  </si>
+  <si>
+    <t>(99, 75, 202, 86)</t>
+  </si>
+  <si>
+    <t>(122, 311, 179, 330)</t>
+  </si>
+  <si>
+    <t>(212, 71, 269, 90)</t>
+  </si>
+  <si>
+    <t>(227, 311, 284, 330)</t>
+  </si>
+  <si>
+    <t>(4, 257, 27, 304)</t>
+  </si>
+  <si>
+    <t>(4, 317, 27, 364)</t>
+  </si>
+  <si>
+    <t>(79, 197, 102, 244)</t>
+  </si>
+  <si>
+    <t>(227, 51, 284, 70)</t>
+  </si>
+  <si>
+    <t>(124, 257, 147, 304)</t>
+  </si>
+  <si>
+    <t>(274, 197, 297, 244)</t>
+  </si>
+  <si>
+    <t>(274, 337, 297, 384)</t>
+  </si>
+  <si>
+    <t>(274, 97, 297, 144)</t>
+  </si>
+  <si>
+    <t>(274, 257, 297, 304)</t>
+  </si>
+  <si>
+    <t>(47, 91, 104, 110)</t>
+  </si>
+  <si>
+    <t>(122, 231, 179, 250)</t>
+  </si>
+  <si>
+    <t>(60.5, 300.5)</t>
+  </si>
+  <si>
+    <t>(135.5, 360.5)</t>
+  </si>
+  <si>
+    <t>(135.5, 380.5)</t>
+  </si>
+  <si>
+    <t>(135.5, 40.5)</t>
+  </si>
+  <si>
+    <t>(105.5, 300.5)</t>
+  </si>
+  <si>
+    <t>(45.5, 220.5)</t>
+  </si>
+  <si>
+    <t>(255.5, 360.5)</t>
+  </si>
+  <si>
+    <t>(120.5, 340.5)</t>
+  </si>
+  <si>
+    <t>(30.5, 120.5)</t>
+  </si>
+  <si>
+    <t>(30.5, 160.5)</t>
+  </si>
+  <si>
+    <t>(120.5, 60.5)</t>
+  </si>
+  <si>
+    <t>(135.5, 20.5)</t>
+  </si>
+  <si>
+    <t>(105.5, 260.5)</t>
+  </si>
+  <si>
+    <t>(60.5, 80.5)</t>
+  </si>
+  <si>
+    <t>(180.5, 340.5)</t>
+  </si>
+  <si>
+    <t>(150.5, 80.5)</t>
+  </si>
+  <si>
+    <t>(150.5, 320.5)</t>
+  </si>
+  <si>
+    <t>(240.5, 80.5)</t>
+  </si>
+  <si>
+    <t>(255.5, 320.5)</t>
+  </si>
+  <si>
+    <t>(15.5, 280.5)</t>
+  </si>
+  <si>
+    <t>(15.5, 340.5)</t>
+  </si>
+  <si>
+    <t>(90.5, 220.5)</t>
+  </si>
+  <si>
+    <t>(255.5, 60.5)</t>
+  </si>
+  <si>
+    <t>(135.5, 280.5)</t>
+  </si>
+  <si>
+    <t>(285.5, 220.5)</t>
+  </si>
+  <si>
+    <t>(285.5, 360.5)</t>
+  </si>
+  <si>
+    <t>(285.5, 120.5)</t>
+  </si>
+  <si>
+    <t>(285.5, 280.5)</t>
+  </si>
+  <si>
+    <t>(75.5, 100.5)</t>
+  </si>
+  <si>
+    <t>(150.5, 240.5)</t>
   </si>
 </sst>
 </file>
@@ -470,13 +563,13 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:C31"/>
+  <dimension ref="A1:D31"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <sheetData>
-    <row r="1" spans="1:3">
+    <row r="1" spans="1:4">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -486,335 +579,428 @@
       <c r="C1" s="1" t="s">
         <v>2</v>
       </c>
-    </row>
-    <row r="2" spans="1:3">
+      <c r="D1" s="1" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="2" spans="1:4">
       <c r="A2">
         <v>1</v>
       </c>
       <c r="B2" t="s">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="C2">
-        <v>1012</v>
-      </c>
-    </row>
-    <row r="3" spans="1:3">
+        <v>4140</v>
+      </c>
+      <c r="D2" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="3" spans="1:4">
       <c r="A3">
         <v>2</v>
       </c>
       <c r="B3" t="s">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="C3">
-        <v>1024</v>
-      </c>
-    </row>
-    <row r="4" spans="1:3">
+        <v>4040</v>
+      </c>
+      <c r="D3" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="4" spans="1:4">
       <c r="A4">
         <v>3</v>
       </c>
       <c r="B4" t="s">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="C4">
-        <v>1024</v>
-      </c>
-    </row>
-    <row r="5" spans="1:3">
+        <v>4040</v>
+      </c>
+      <c r="D4" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="5" spans="1:4">
       <c r="A5">
         <v>4</v>
       </c>
       <c r="B5" t="s">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="C5">
-        <v>1012</v>
-      </c>
-    </row>
-    <row r="6" spans="1:3">
+        <v>4040</v>
+      </c>
+      <c r="D5" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="6" spans="1:4">
       <c r="A6">
         <v>5</v>
       </c>
       <c r="B6" t="s">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="C6">
-        <v>1012</v>
-      </c>
-    </row>
-    <row r="7" spans="1:3">
+        <v>1024</v>
+      </c>
+      <c r="D6" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="7" spans="1:4">
       <c r="A7">
         <v>6</v>
       </c>
       <c r="B7" t="s">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="C7">
-        <v>1012</v>
-      </c>
-    </row>
-    <row r="8" spans="1:3">
+        <v>4096</v>
+      </c>
+      <c r="D7" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="8" spans="1:4">
       <c r="A8">
         <v>7</v>
       </c>
       <c r="B8" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="C8">
-        <v>1012</v>
-      </c>
-    </row>
-    <row r="9" spans="1:3">
+        <v>1024</v>
+      </c>
+      <c r="D8" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="9" spans="1:4">
       <c r="A9">
         <v>8</v>
       </c>
       <c r="B9" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="C9">
-        <v>1012</v>
-      </c>
-    </row>
-    <row r="10" spans="1:3">
+        <v>1008</v>
+      </c>
+      <c r="D9" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="10" spans="1:4">
       <c r="A10">
         <v>9</v>
       </c>
       <c r="B10" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="C10">
         <v>1012</v>
       </c>
-    </row>
-    <row r="11" spans="1:3">
+      <c r="D10" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="11" spans="1:4">
       <c r="A11">
         <v>10</v>
       </c>
       <c r="B11" t="s">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="C11">
-        <v>1012</v>
-      </c>
-    </row>
-    <row r="12" spans="1:3">
+        <v>1024</v>
+      </c>
+      <c r="D11" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="12" spans="1:4">
       <c r="A12">
         <v>11</v>
       </c>
       <c r="B12" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="C12">
-        <v>1024</v>
-      </c>
-    </row>
-    <row r="13" spans="1:3">
+        <v>4040</v>
+      </c>
+      <c r="D12" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="13" spans="1:4">
       <c r="A13">
         <v>12</v>
       </c>
       <c r="B13" t="s">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="C13">
-        <v>1012</v>
-      </c>
-    </row>
-    <row r="14" spans="1:3">
+        <v>4040</v>
+      </c>
+      <c r="D13" t="s">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="14" spans="1:4">
       <c r="A14">
         <v>13</v>
       </c>
       <c r="B14" t="s">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="C14">
-        <v>1012</v>
-      </c>
-    </row>
-    <row r="15" spans="1:3">
+        <v>1024</v>
+      </c>
+      <c r="D14" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="15" spans="1:4">
       <c r="A15">
         <v>14</v>
       </c>
       <c r="B15" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="C15">
-        <v>1012</v>
-      </c>
-    </row>
-    <row r="16" spans="1:3">
+        <v>1008</v>
+      </c>
+      <c r="D15" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="16" spans="1:4">
       <c r="A16">
         <v>15</v>
       </c>
       <c r="B16" t="s">
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="C16">
-        <v>1012</v>
-      </c>
-    </row>
-    <row r="17" spans="1:3">
+        <v>1008</v>
+      </c>
+      <c r="D16" t="s">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="17" spans="1:4">
       <c r="A17">
         <v>16</v>
       </c>
       <c r="B17" t="s">
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="C17">
-        <v>1012</v>
-      </c>
-    </row>
-    <row r="18" spans="1:3">
+        <v>1020</v>
+      </c>
+      <c r="D17" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="18" spans="1:4">
       <c r="A18">
         <v>17</v>
       </c>
       <c r="B18" t="s">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="C18">
         <v>1008</v>
       </c>
-    </row>
-    <row r="19" spans="1:3">
+      <c r="D18" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="19" spans="1:4">
       <c r="A19">
         <v>18</v>
       </c>
       <c r="B19" t="s">
-        <v>20</v>
+        <v>21</v>
       </c>
       <c r="C19">
-        <v>1012</v>
-      </c>
-    </row>
-    <row r="20" spans="1:3">
+        <v>1008</v>
+      </c>
+      <c r="D19" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="20" spans="1:4">
       <c r="A20">
         <v>19</v>
       </c>
       <c r="B20" t="s">
-        <v>21</v>
+        <v>22</v>
       </c>
       <c r="C20">
         <v>1008</v>
       </c>
-    </row>
-    <row r="21" spans="1:3">
+      <c r="D20" t="s">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="21" spans="1:4">
       <c r="A21">
         <v>20</v>
       </c>
       <c r="B21" t="s">
-        <v>22</v>
+        <v>23</v>
       </c>
       <c r="C21">
-        <v>1008</v>
-      </c>
-    </row>
-    <row r="22" spans="1:3">
+        <v>1012</v>
+      </c>
+      <c r="D21" t="s">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="22" spans="1:4">
       <c r="A22">
         <v>21</v>
       </c>
       <c r="B22" t="s">
-        <v>23</v>
+        <v>24</v>
       </c>
       <c r="C22">
-        <v>1008</v>
-      </c>
-    </row>
-    <row r="23" spans="1:3">
+        <v>1012</v>
+      </c>
+      <c r="D22" t="s">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="23" spans="1:4">
       <c r="A23">
         <v>22</v>
       </c>
       <c r="B23" t="s">
-        <v>24</v>
+        <v>25</v>
       </c>
       <c r="C23">
-        <v>1008</v>
-      </c>
-    </row>
-    <row r="24" spans="1:3">
+        <v>1012</v>
+      </c>
+      <c r="D23" t="s">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="24" spans="1:4">
       <c r="A24">
         <v>23</v>
       </c>
       <c r="B24" t="s">
-        <v>25</v>
+        <v>26</v>
       </c>
       <c r="C24">
         <v>1008</v>
       </c>
-    </row>
-    <row r="25" spans="1:3">
+      <c r="D24" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="25" spans="1:4">
       <c r="A25">
         <v>24</v>
       </c>
       <c r="B25" t="s">
-        <v>26</v>
+        <v>27</v>
       </c>
       <c r="C25">
-        <v>1008</v>
-      </c>
-    </row>
-    <row r="26" spans="1:3">
+        <v>1012</v>
+      </c>
+      <c r="D25" t="s">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="26" spans="1:4">
       <c r="A26">
         <v>25</v>
       </c>
       <c r="B26" t="s">
-        <v>27</v>
+        <v>28</v>
       </c>
       <c r="C26">
-        <v>1020</v>
-      </c>
-    </row>
-    <row r="27" spans="1:3">
+        <v>1012</v>
+      </c>
+      <c r="D26" t="s">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="27" spans="1:4">
       <c r="A27">
         <v>26</v>
       </c>
       <c r="B27" t="s">
-        <v>28</v>
+        <v>29</v>
       </c>
       <c r="C27">
-        <v>1020</v>
-      </c>
-    </row>
-    <row r="28" spans="1:3">
+        <v>1012</v>
+      </c>
+      <c r="D27" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="28" spans="1:4">
       <c r="A28">
         <v>27</v>
       </c>
       <c r="B28" t="s">
-        <v>29</v>
+        <v>30</v>
       </c>
       <c r="C28">
-        <v>1008</v>
-      </c>
-    </row>
-    <row r="29" spans="1:3">
+        <v>1012</v>
+      </c>
+      <c r="D28" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="29" spans="1:4">
       <c r="A29">
         <v>28</v>
       </c>
       <c r="B29" t="s">
-        <v>30</v>
+        <v>31</v>
       </c>
       <c r="C29">
-        <v>1024</v>
-      </c>
-    </row>
-    <row r="30" spans="1:3">
+        <v>1012</v>
+      </c>
+      <c r="D29" t="s">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="30" spans="1:4">
       <c r="A30">
         <v>29</v>
       </c>
       <c r="B30" t="s">
-        <v>31</v>
+        <v>32</v>
       </c>
       <c r="C30">
-        <v>1012</v>
-      </c>
-    </row>
-    <row r="31" spans="1:3">
+        <v>1008</v>
+      </c>
+      <c r="D30" t="s">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="31" spans="1:4">
       <c r="A31">
         <v>30</v>
       </c>
       <c r="B31" t="s">
-        <v>32</v>
+        <v>33</v>
       </c>
       <c r="C31">
-        <v>1012</v>
+        <v>1008</v>
+      </c>
+      <c r="D31" t="s">
+        <v>63</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
removing already experimented parts
</commit_message>
<xml_diff>
--- a/display/smooth_region_coordinates.xlsx
+++ b/display/smooth_region_coordinates.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="64" uniqueCount="64">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="33" uniqueCount="33">
   <si>
     <t>Region</t>
   </si>
@@ -25,9 +25,6 @@
     <t>Area</t>
   </si>
   <si>
-    <t>Centroid</t>
-  </si>
-  <si>
     <t>(37, 255, 84, 346)</t>
   </si>
   <si>
@@ -116,96 +113,6 @@
   </si>
   <si>
     <t>(122, 231, 179, 250)</t>
-  </si>
-  <si>
-    <t>(60.5, 300.5)</t>
-  </si>
-  <si>
-    <t>(135.5, 360.5)</t>
-  </si>
-  <si>
-    <t>(135.5, 380.5)</t>
-  </si>
-  <si>
-    <t>(135.5, 40.5)</t>
-  </si>
-  <si>
-    <t>(105.5, 300.5)</t>
-  </si>
-  <si>
-    <t>(45.5, 220.5)</t>
-  </si>
-  <si>
-    <t>(255.5, 360.5)</t>
-  </si>
-  <si>
-    <t>(120.5, 340.5)</t>
-  </si>
-  <si>
-    <t>(30.5, 120.5)</t>
-  </si>
-  <si>
-    <t>(30.5, 160.5)</t>
-  </si>
-  <si>
-    <t>(120.5, 60.5)</t>
-  </si>
-  <si>
-    <t>(135.5, 20.5)</t>
-  </si>
-  <si>
-    <t>(105.5, 260.5)</t>
-  </si>
-  <si>
-    <t>(60.5, 80.5)</t>
-  </si>
-  <si>
-    <t>(180.5, 340.5)</t>
-  </si>
-  <si>
-    <t>(150.5, 80.5)</t>
-  </si>
-  <si>
-    <t>(150.5, 320.5)</t>
-  </si>
-  <si>
-    <t>(240.5, 80.5)</t>
-  </si>
-  <si>
-    <t>(255.5, 320.5)</t>
-  </si>
-  <si>
-    <t>(15.5, 280.5)</t>
-  </si>
-  <si>
-    <t>(15.5, 340.5)</t>
-  </si>
-  <si>
-    <t>(90.5, 220.5)</t>
-  </si>
-  <si>
-    <t>(255.5, 60.5)</t>
-  </si>
-  <si>
-    <t>(135.5, 280.5)</t>
-  </si>
-  <si>
-    <t>(285.5, 220.5)</t>
-  </si>
-  <si>
-    <t>(285.5, 360.5)</t>
-  </si>
-  <si>
-    <t>(285.5, 120.5)</t>
-  </si>
-  <si>
-    <t>(285.5, 280.5)</t>
-  </si>
-  <si>
-    <t>(75.5, 100.5)</t>
-  </si>
-  <si>
-    <t>(150.5, 240.5)</t>
   </si>
 </sst>
 </file>
@@ -563,13 +470,13 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:D31"/>
+  <dimension ref="A1:C31"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <sheetData>
-    <row r="1" spans="1:4">
+    <row r="1" spans="1:3">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -579,428 +486,335 @@
       <c r="C1" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="1" t="s">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="2" spans="1:4">
+    </row>
+    <row r="2" spans="1:3">
       <c r="A2">
         <v>1</v>
       </c>
       <c r="B2" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="C2">
         <v>4140</v>
       </c>
-      <c r="D2" t="s">
-        <v>34</v>
-      </c>
-    </row>
-    <row r="3" spans="1:4">
+    </row>
+    <row r="3" spans="1:3">
       <c r="A3">
         <v>2</v>
       </c>
       <c r="B3" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="C3">
         <v>4040</v>
       </c>
-      <c r="D3" t="s">
-        <v>35</v>
-      </c>
-    </row>
-    <row r="4" spans="1:4">
+    </row>
+    <row r="4" spans="1:3">
       <c r="A4">
         <v>3</v>
       </c>
       <c r="B4" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="C4">
         <v>4040</v>
       </c>
-      <c r="D4" t="s">
-        <v>36</v>
-      </c>
-    </row>
-    <row r="5" spans="1:4">
+    </row>
+    <row r="5" spans="1:3">
       <c r="A5">
         <v>4</v>
       </c>
       <c r="B5" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="C5">
         <v>4040</v>
       </c>
-      <c r="D5" t="s">
-        <v>37</v>
-      </c>
-    </row>
-    <row r="6" spans="1:4">
+    </row>
+    <row r="6" spans="1:3">
       <c r="A6">
         <v>5</v>
       </c>
       <c r="B6" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="C6">
         <v>1024</v>
       </c>
-      <c r="D6" t="s">
-        <v>38</v>
-      </c>
-    </row>
-    <row r="7" spans="1:4">
+    </row>
+    <row r="7" spans="1:3">
       <c r="A7">
         <v>6</v>
       </c>
       <c r="B7" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="C7">
         <v>4096</v>
       </c>
-      <c r="D7" t="s">
-        <v>39</v>
-      </c>
-    </row>
-    <row r="8" spans="1:4">
+    </row>
+    <row r="8" spans="1:3">
       <c r="A8">
         <v>7</v>
       </c>
       <c r="B8" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="C8">
         <v>1024</v>
       </c>
-      <c r="D8" t="s">
-        <v>40</v>
-      </c>
-    </row>
-    <row r="9" spans="1:4">
+    </row>
+    <row r="9" spans="1:3">
       <c r="A9">
         <v>8</v>
       </c>
       <c r="B9" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="C9">
         <v>1008</v>
       </c>
-      <c r="D9" t="s">
-        <v>41</v>
-      </c>
-    </row>
-    <row r="10" spans="1:4">
+    </row>
+    <row r="10" spans="1:3">
       <c r="A10">
         <v>9</v>
       </c>
       <c r="B10" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="C10">
         <v>1012</v>
       </c>
-      <c r="D10" t="s">
-        <v>42</v>
-      </c>
-    </row>
-    <row r="11" spans="1:4">
+    </row>
+    <row r="11" spans="1:3">
       <c r="A11">
         <v>10</v>
       </c>
       <c r="B11" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="C11">
         <v>1024</v>
       </c>
-      <c r="D11" t="s">
-        <v>43</v>
-      </c>
-    </row>
-    <row r="12" spans="1:4">
+    </row>
+    <row r="12" spans="1:3">
       <c r="A12">
         <v>11</v>
       </c>
       <c r="B12" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="C12">
         <v>4040</v>
       </c>
-      <c r="D12" t="s">
-        <v>44</v>
-      </c>
-    </row>
-    <row r="13" spans="1:4">
+    </row>
+    <row r="13" spans="1:3">
       <c r="A13">
         <v>12</v>
       </c>
       <c r="B13" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="C13">
         <v>4040</v>
       </c>
-      <c r="D13" t="s">
-        <v>45</v>
-      </c>
-    </row>
-    <row r="14" spans="1:4">
+    </row>
+    <row r="14" spans="1:3">
       <c r="A14">
         <v>13</v>
       </c>
       <c r="B14" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="C14">
         <v>1024</v>
       </c>
-      <c r="D14" t="s">
-        <v>46</v>
-      </c>
-    </row>
-    <row r="15" spans="1:4">
+    </row>
+    <row r="15" spans="1:3">
       <c r="A15">
         <v>14</v>
       </c>
       <c r="B15" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="C15">
         <v>1008</v>
       </c>
-      <c r="D15" t="s">
-        <v>47</v>
-      </c>
-    </row>
-    <row r="16" spans="1:4">
+    </row>
+    <row r="16" spans="1:3">
       <c r="A16">
         <v>15</v>
       </c>
       <c r="B16" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="C16">
         <v>1008</v>
       </c>
-      <c r="D16" t="s">
-        <v>48</v>
-      </c>
-    </row>
-    <row r="17" spans="1:4">
+    </row>
+    <row r="17" spans="1:3">
       <c r="A17">
         <v>16</v>
       </c>
       <c r="B17" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="C17">
         <v>1020</v>
       </c>
-      <c r="D17" t="s">
-        <v>49</v>
-      </c>
-    </row>
-    <row r="18" spans="1:4">
+    </row>
+    <row r="18" spans="1:3">
       <c r="A18">
         <v>17</v>
       </c>
       <c r="B18" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="C18">
         <v>1008</v>
       </c>
-      <c r="D18" t="s">
-        <v>50</v>
-      </c>
-    </row>
-    <row r="19" spans="1:4">
+    </row>
+    <row r="19" spans="1:3">
       <c r="A19">
         <v>18</v>
       </c>
       <c r="B19" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="C19">
         <v>1008</v>
       </c>
-      <c r="D19" t="s">
-        <v>51</v>
-      </c>
-    </row>
-    <row r="20" spans="1:4">
+    </row>
+    <row r="20" spans="1:3">
       <c r="A20">
         <v>19</v>
       </c>
       <c r="B20" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="C20">
         <v>1008</v>
       </c>
-      <c r="D20" t="s">
-        <v>52</v>
-      </c>
-    </row>
-    <row r="21" spans="1:4">
+    </row>
+    <row r="21" spans="1:3">
       <c r="A21">
         <v>20</v>
       </c>
       <c r="B21" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="C21">
         <v>1012</v>
       </c>
-      <c r="D21" t="s">
-        <v>53</v>
-      </c>
-    </row>
-    <row r="22" spans="1:4">
+    </row>
+    <row r="22" spans="1:3">
       <c r="A22">
         <v>21</v>
       </c>
       <c r="B22" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="C22">
         <v>1012</v>
       </c>
-      <c r="D22" t="s">
-        <v>54</v>
-      </c>
-    </row>
-    <row r="23" spans="1:4">
+    </row>
+    <row r="23" spans="1:3">
       <c r="A23">
         <v>22</v>
       </c>
       <c r="B23" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="C23">
         <v>1012</v>
       </c>
-      <c r="D23" t="s">
-        <v>55</v>
-      </c>
-    </row>
-    <row r="24" spans="1:4">
+    </row>
+    <row r="24" spans="1:3">
       <c r="A24">
         <v>23</v>
       </c>
       <c r="B24" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="C24">
         <v>1008</v>
       </c>
-      <c r="D24" t="s">
-        <v>56</v>
-      </c>
-    </row>
-    <row r="25" spans="1:4">
+    </row>
+    <row r="25" spans="1:3">
       <c r="A25">
         <v>24</v>
       </c>
       <c r="B25" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="C25">
         <v>1012</v>
       </c>
-      <c r="D25" t="s">
-        <v>57</v>
-      </c>
-    </row>
-    <row r="26" spans="1:4">
+    </row>
+    <row r="26" spans="1:3">
       <c r="A26">
         <v>25</v>
       </c>
       <c r="B26" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="C26">
         <v>1012</v>
       </c>
-      <c r="D26" t="s">
-        <v>58</v>
-      </c>
-    </row>
-    <row r="27" spans="1:4">
+    </row>
+    <row r="27" spans="1:3">
       <c r="A27">
         <v>26</v>
       </c>
       <c r="B27" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="C27">
         <v>1012</v>
       </c>
-      <c r="D27" t="s">
-        <v>59</v>
-      </c>
-    </row>
-    <row r="28" spans="1:4">
+    </row>
+    <row r="28" spans="1:3">
       <c r="A28">
         <v>27</v>
       </c>
       <c r="B28" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="C28">
         <v>1012</v>
       </c>
-      <c r="D28" t="s">
-        <v>60</v>
-      </c>
-    </row>
-    <row r="29" spans="1:4">
+    </row>
+    <row r="29" spans="1:3">
       <c r="A29">
         <v>28</v>
       </c>
       <c r="B29" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="C29">
         <v>1012</v>
       </c>
-      <c r="D29" t="s">
-        <v>61</v>
-      </c>
-    </row>
-    <row r="30" spans="1:4">
+    </row>
+    <row r="30" spans="1:3">
       <c r="A30">
         <v>29</v>
       </c>
       <c r="B30" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="C30">
         <v>1008</v>
       </c>
-      <c r="D30" t="s">
-        <v>62</v>
-      </c>
-    </row>
-    <row r="31" spans="1:4">
+    </row>
+    <row r="31" spans="1:3">
       <c r="A31">
         <v>30</v>
       </c>
       <c r="B31" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="C31">
         <v>1008</v>
-      </c>
-      <c r="D31" t="s">
-        <v>63</v>
       </c>
     </row>
   </sheetData>

</xml_diff>